<commit_message>
Change all spreadsheet timeout values to 6 or 7 seconds vice 6000 or 7000 seconds. Add comment to spreadsheets where timeout values are specified that timeout values are seconds, not milliseconds:
Default wait time was set to 7000, and in some steps we were passing 6000. 

Per https://seleniumhq.github.io/selenium/docs/api/java/org/openqa/selenium/support/ui/WebDriverWait.html
-> WebDriverWait(WebDriver driver, long timeOutInSeconds)

That's seconds, not milliseconds. 6000 and 7000 are 100 minutes and 116 minutes respectively.
</commit_message>
<xml_diff>
--- a/example_usage/suites/excel_csv.xlsx
+++ b/example_usage/suites/excel_csv.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felala\Documents\demo_back\component\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5829FB2-0636-41F7-A6B7-DC8E7EBAAE2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>key</t>
   </si>
@@ -108,18 +109,12 @@
     <t>Windows</t>
   </si>
   <si>
-    <t>Plateform type for remote web driver intializing</t>
-  </si>
-  <si>
     <t>webdriver.version.chrome</t>
   </si>
   <si>
     <t>61.0</t>
   </si>
   <si>
-    <t>Version for plateform type selected</t>
-  </si>
-  <si>
     <t>webdriver.platform.ie</t>
   </si>
   <si>
@@ -177,9 +172,6 @@
     <t>webdriver.e34:per_test_timeout_ms</t>
   </si>
   <si>
-    <t>7000</t>
-  </si>
-  <si>
     <t>testdata.filename</t>
   </si>
   <si>
@@ -196,12 +188,24 @@
   </si>
   <si>
     <t>test.alpha</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Wait time delay is seconds, not milliseconds</t>
+  </si>
+  <si>
+    <t>Version for platform type selected</t>
+  </si>
+  <si>
+    <t>Platform type for remote web driver intializing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -585,22 +589,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="4"/>
+    <col min="3" max="3" width="62.42578125" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -611,7 +615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -622,7 +626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -633,7 +637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -644,7 +648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
@@ -655,7 +659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -666,7 +670,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -674,155 +678,158 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="C13" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="C14" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="11"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="11"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="11"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="11"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="11"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -832,25 +839,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -874,7 +881,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -886,15 +893,15 @@
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" s="10"/>
       <c r="G3" s="2"/>

</xml_diff>